<commit_message>
update labor cost dataset and planning
</commit_message>
<xml_diff>
--- a/Gantt.xlsx
+++ b/Gantt.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Monash University LPDP\Study\2024 - Term 5\ITI5057 - Project Management\Assessment 1\Risk Analysis\Monash-PM-Assignment-Monte-Carlo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0A2AEBC-7FB8-4D97-B1B3-F5FE58CAD07E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE7A3EFA-4CB8-439E-95D5-445DAF026F90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{0102A14C-CF0C-4EBD-81A6-EA651CF50D0E}"/>
   </bookViews>
   <sheets>
     <sheet name="cost reference" sheetId="2" r:id="rId1"/>
-    <sheet name="Gantt" sheetId="7" r:id="rId2"/>
+    <sheet name="Gantt" sheetId="10" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,10 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="22">
-  <si>
-    <t>Month</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="26">
   <si>
     <t>Cost Incurred</t>
   </si>
@@ -48,9 +45,6 @@
     <t>Total Period</t>
   </si>
   <si>
-    <t>B. Data Modelling</t>
-  </si>
-  <si>
     <t>Year</t>
   </si>
   <si>
@@ -75,6 +69,9 @@
     <t>System Analyst</t>
   </si>
   <si>
+    <t>Business Analyst</t>
+  </si>
+  <si>
     <t>Project Manager</t>
   </si>
   <si>
@@ -84,6 +81,9 @@
     <t>Data Engineer</t>
   </si>
   <si>
+    <t>BI Developer</t>
+  </si>
+  <si>
     <t>v</t>
   </si>
   <si>
@@ -91,12 +91,6 @@
   </si>
   <si>
     <t>Total Cost</t>
-  </si>
-  <si>
-    <t>C. Solution Development and Deployment</t>
-  </si>
-  <si>
-    <t>D. User Acceptance Testing</t>
   </si>
   <si>
     <t>A. Requirement Definition, System Design and Data Preparation</t>
@@ -104,6 +98,24 @@
   <si>
     <t>Development Phase 
 and Resource Deployment</t>
+  </si>
+  <si>
+    <t>Total Labor Cost</t>
+  </si>
+  <si>
+    <t>Contingency Reserve</t>
+  </si>
+  <si>
+    <t>B. Data Modelling, Solution Development and Deployment</t>
+  </si>
+  <si>
+    <t>C. User Acceptance Testing</t>
+  </si>
+  <si>
+    <t>Week</t>
+  </si>
+  <si>
+    <t>Superannuation Adjustment</t>
   </si>
 </sst>
 </file>
@@ -174,7 +186,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -192,6 +204,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -538,10 +552,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8ED9E01A-EE7F-4169-9FAA-B4D3D08D7FCA}">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="C8" sqref="C8:E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -555,25 +569,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>6</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>7</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>8</v>
-      </c>
-      <c r="F1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
@@ -581,7 +595,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C2">
         <v>700</v>
@@ -601,16 +615,16 @@
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C3">
+        <v>775</v>
+      </c>
+      <c r="D3">
+        <v>550</v>
+      </c>
+      <c r="E3">
         <v>900</v>
-      </c>
-      <c r="D3">
-        <v>800</v>
-      </c>
-      <c r="E3">
-        <v>1100</v>
       </c>
       <c r="F3">
         <v>1</v>
@@ -621,13 +635,13 @@
         <v>0</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C4">
         <v>900</v>
       </c>
       <c r="D4">
-        <v>700</v>
+        <v>800</v>
       </c>
       <c r="E4">
         <v>1100</v>
@@ -641,16 +655,16 @@
         <v>0</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C5">
-        <v>800</v>
+        <v>900</v>
       </c>
       <c r="D5">
-        <v>650</v>
+        <v>700</v>
       </c>
       <c r="E5">
-        <v>1050</v>
+        <v>1100</v>
       </c>
       <c r="F5">
         <v>1</v>
@@ -661,18 +675,58 @@
         <v>0</v>
       </c>
       <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6">
+        <v>800</v>
+      </c>
+      <c r="D6">
+        <v>650</v>
+      </c>
+      <c r="E6">
+        <v>1050</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>0</v>
+      </c>
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7">
+        <v>775</v>
+      </c>
+      <c r="D7">
+        <v>600</v>
+      </c>
+      <c r="E7">
+        <v>900</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>0</v>
+      </c>
+      <c r="B8" t="s">
         <v>16</v>
       </c>
-      <c r="C6">
+      <c r="C8">
         <v>1000</v>
       </c>
-      <c r="D6">
+      <c r="D8">
         <v>800</v>
       </c>
-      <c r="E6">
+      <c r="E8">
         <v>1300</v>
       </c>
-      <c r="F6">
+      <c r="F8">
         <v>1</v>
       </c>
     </row>
@@ -682,11 +736,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F3D5CE3-4E87-4FBC-AEDA-D1014D2BB096}">
-  <dimension ref="B2:Q19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01DE9161-96AE-434B-951E-00EFF3491272}">
+  <dimension ref="B2:V19"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="AL17" sqref="AL17"/>
+      <selection activeCell="AK11" sqref="AK11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -701,19 +755,18 @@
     <col min="9" max="9" width="2.90625" customWidth="1"/>
     <col min="10" max="10" width="3.08984375" customWidth="1"/>
     <col min="11" max="11" width="2.81640625" customWidth="1"/>
-    <col min="12" max="12" width="3.54296875" customWidth="1"/>
-    <col min="13" max="15" width="2.90625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="6.90625" customWidth="1"/>
-    <col min="17" max="17" width="9.453125" customWidth="1"/>
+    <col min="12" max="12" width="6.90625" customWidth="1"/>
+    <col min="13" max="13" width="9.453125" customWidth="1"/>
+    <col min="14" max="14" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:17" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:22" x14ac:dyDescent="0.35">
       <c r="B2" s="7" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C2" s="7"/>
       <c r="D2" s="6" t="s">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
@@ -722,18 +775,17 @@
       <c r="I2" s="6"/>
       <c r="J2" s="6"/>
       <c r="K2" s="6"/>
-      <c r="L2" s="6"/>
-      <c r="M2" s="6"/>
-      <c r="N2" s="6"/>
-      <c r="O2" s="6"/>
-      <c r="P2" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q2" s="7" t="s">
+      <c r="L2" s="7" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="M2" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="N2" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="2:22" x14ac:dyDescent="0.35">
       <c r="B3" s="7"/>
       <c r="C3" s="7"/>
       <c r="D3" s="1">
@@ -760,24 +812,13 @@
       <c r="K3" s="1">
         <v>8</v>
       </c>
-      <c r="L3" s="1">
-        <v>9</v>
-      </c>
-      <c r="M3" s="1">
-        <v>10</v>
-      </c>
-      <c r="N3" s="1">
-        <v>11</v>
-      </c>
-      <c r="O3" s="1">
-        <v>12</v>
-      </c>
-      <c r="P3" s="7"/>
-      <c r="Q3" s="7"/>
-    </row>
-    <row r="4" spans="2:17" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="L3" s="7"/>
+      <c r="M3" s="7"/>
+      <c r="N3" s="7"/>
+    </row>
+    <row r="4" spans="2:22" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B4" s="8" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C4" s="8"/>
       <c r="D4" s="2"/>
@@ -791,96 +832,108 @@
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
-      <c r="O4" s="2"/>
-      <c r="P4" s="2"/>
-      <c r="Q4" s="2"/>
-    </row>
-    <row r="5" spans="2:17" x14ac:dyDescent="0.35">
+    </row>
+    <row r="5" spans="2:22" x14ac:dyDescent="0.35">
       <c r="B5" s="2"/>
       <c r="C5" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
+      <c r="E5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>15</v>
+      </c>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
-      <c r="L5" s="2"/>
-      <c r="M5" s="2"/>
-      <c r="N5" s="2"/>
-      <c r="O5" s="2"/>
-      <c r="P5" s="2">
-        <v>18</v>
-      </c>
-      <c r="Q5" s="3">
-        <f>VLOOKUP(C5,'cost reference'!$B$2:$C$6,2,0)*P5*1.115</f>
-        <v>18063</v>
-      </c>
-    </row>
-    <row r="6" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="L5" s="2">
+        <f>COUNTA(D5:K5)*5</f>
+        <v>15</v>
+      </c>
+      <c r="M5" s="3">
+        <f>VLOOKUP(C5,'cost reference'!$B$2:$C$8,2,0)*L5</f>
+        <v>13500</v>
+      </c>
+      <c r="N5" s="3">
+        <f>1.115*M5</f>
+        <v>15052.5</v>
+      </c>
+    </row>
+    <row r="6" spans="2:22" x14ac:dyDescent="0.35">
       <c r="B6" s="2"/>
       <c r="C6" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
+      <c r="E6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>15</v>
+      </c>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
-      <c r="L6" s="2"/>
-      <c r="M6" s="2"/>
-      <c r="N6" s="2"/>
-      <c r="O6" s="2"/>
-      <c r="P6" s="2">
-        <v>18</v>
-      </c>
-      <c r="Q6" s="3">
-        <f>VLOOKUP(C6,'cost reference'!$B$2:$C$6,2,0)*P6*1.115</f>
-        <v>14049</v>
-      </c>
-    </row>
-    <row r="7" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="L6" s="2">
+        <f t="shared" ref="L6:L16" si="0">COUNTA(D6:K6)*5</f>
+        <v>15</v>
+      </c>
+      <c r="M6" s="3">
+        <f>VLOOKUP(C6,'cost reference'!$B$2:$C$8,2,0)*L6</f>
+        <v>10500</v>
+      </c>
+      <c r="N6" s="3">
+        <f t="shared" ref="N6:N16" si="1">1.115*M6</f>
+        <v>11707.5</v>
+      </c>
+    </row>
+    <row r="7" spans="2:22" x14ac:dyDescent="0.35">
       <c r="B7" s="2"/>
       <c r="C7" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
+      <c r="E7" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>15</v>
+      </c>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
-      <c r="L7" s="2"/>
-      <c r="M7" s="2"/>
-      <c r="N7" s="2"/>
-      <c r="O7" s="2"/>
-      <c r="P7" s="2">
-        <v>18</v>
-      </c>
-      <c r="Q7" s="3">
-        <f>VLOOKUP(C7,'cost reference'!$B$2:$C$6,2,0)*P7*1.115</f>
-        <v>16056</v>
-      </c>
-    </row>
-    <row r="8" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="B8" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C8" s="5"/>
+      <c r="L7" s="2">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="M7" s="3">
+        <f>VLOOKUP(C7,'cost reference'!$B$2:$C$8,2,0)*L7</f>
+        <v>12000</v>
+      </c>
+      <c r="N7" s="3">
+        <f t="shared" si="1"/>
+        <v>13380</v>
+      </c>
+    </row>
+    <row r="8" spans="2:22" ht="29.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B8" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="8"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
@@ -890,205 +943,233 @@
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
-      <c r="M8" s="2"/>
-      <c r="N8" s="2"/>
-      <c r="O8" s="2"/>
-      <c r="P8" s="2"/>
-      <c r="Q8" s="3"/>
-    </row>
-    <row r="9" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="M8" s="3"/>
+      <c r="N8" s="3"/>
+    </row>
+    <row r="9" spans="2:22" x14ac:dyDescent="0.35">
       <c r="B9" s="2"/>
       <c r="C9" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D9" s="2"/>
-      <c r="E9" s="2" t="s">
-        <v>15</v>
-      </c>
+      <c r="E9" s="2"/>
       <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
+      <c r="G9" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>15</v>
+      </c>
       <c r="K9" s="2"/>
-      <c r="L9" s="2"/>
-      <c r="M9" s="2"/>
-      <c r="N9" s="2"/>
-      <c r="O9" s="2"/>
-      <c r="P9" s="2">
-        <f t="shared" ref="P6:P15" si="0">COUNTA(D9:O9)*20</f>
+      <c r="L9" s="2">
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="Q9" s="3">
-        <f>VLOOKUP(C9,'cost reference'!$B$2:$C$6,2,0)*P9*1.115</f>
+      <c r="M9" s="3">
+        <f>VLOOKUP(C9,'cost reference'!$B$2:$C$8,2,0)*L9</f>
+        <v>18000</v>
+      </c>
+      <c r="N9" s="3">
+        <f t="shared" si="1"/>
         <v>20070</v>
       </c>
-    </row>
-    <row r="10" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="V9" s="9"/>
+    </row>
+    <row r="10" spans="2:22" x14ac:dyDescent="0.35">
       <c r="B10" s="2"/>
       <c r="C10" s="2" t="s">
         <v>16</v>
       </c>
       <c r="D10" s="2"/>
-      <c r="E10" s="2" t="s">
-        <v>15</v>
-      </c>
+      <c r="E10" s="2"/>
       <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
+      <c r="G10" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>15</v>
+      </c>
       <c r="K10" s="2"/>
-      <c r="L10" s="2"/>
-      <c r="M10" s="2"/>
-      <c r="N10" s="2"/>
-      <c r="O10" s="2"/>
-      <c r="P10" s="2">
+      <c r="L10" s="2">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="Q10" s="3">
-        <f>VLOOKUP(C10,'cost reference'!$B$2:$C$6,2,0)*P10*1.115</f>
+      <c r="M10" s="3">
+        <f>VLOOKUP(C10,'cost reference'!$B$2:$C$8,2,0)*L10</f>
+        <v>20000</v>
+      </c>
+      <c r="N10" s="3">
+        <f t="shared" si="1"/>
         <v>22300</v>
       </c>
-    </row>
-    <row r="11" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="V10" s="9"/>
+    </row>
+    <row r="11" spans="2:22" x14ac:dyDescent="0.35">
       <c r="B11" s="2"/>
       <c r="C11" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D11" s="2"/>
-      <c r="E11" s="2" t="s">
-        <v>15</v>
-      </c>
+      <c r="E11" s="2"/>
       <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
-      <c r="J11" s="2"/>
+      <c r="G11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>15</v>
+      </c>
       <c r="K11" s="2"/>
-      <c r="L11" s="2"/>
-      <c r="M11" s="2"/>
-      <c r="N11" s="2"/>
-      <c r="O11" s="2"/>
-      <c r="P11" s="2">
+      <c r="L11" s="2">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="Q11" s="3">
-        <f>VLOOKUP(C11,'cost reference'!$B$2:$C$6,2,0)*P11*1.115</f>
+      <c r="M11" s="3">
+        <f>VLOOKUP(C11,'cost reference'!$B$2:$C$8,2,0)*L11</f>
+        <v>16000</v>
+      </c>
+      <c r="N11" s="3">
+        <f t="shared" si="1"/>
         <v>17840</v>
       </c>
     </row>
-    <row r="12" spans="2:17" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="C12" s="8"/>
+    <row r="12" spans="2:22" x14ac:dyDescent="0.35">
+      <c r="B12" s="2"/>
+      <c r="C12" s="2" t="s">
+        <v>9</v>
+      </c>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
-      <c r="J12" s="2"/>
+      <c r="G12" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>15</v>
+      </c>
       <c r="K12" s="2"/>
-      <c r="L12" s="2"/>
-      <c r="M12" s="2"/>
-      <c r="N12" s="2"/>
-      <c r="O12" s="2"/>
-      <c r="P12" s="2"/>
-      <c r="Q12" s="3"/>
-    </row>
-    <row r="13" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="L12" s="2">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="M12" s="3">
+        <f>VLOOKUP(C12,'cost reference'!$B$2:$C$8,2,0)*L12</f>
+        <v>14000</v>
+      </c>
+      <c r="N12" s="3">
+        <f t="shared" si="1"/>
+        <v>15610</v>
+      </c>
+      <c r="V12" s="9"/>
+    </row>
+    <row r="13" spans="2:22" x14ac:dyDescent="0.35">
       <c r="B13" s="2"/>
       <c r="C13" s="2" t="s">
         <v>12</v>
       </c>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
-      <c r="F13" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
-      <c r="J13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>15</v>
+      </c>
       <c r="K13" s="2"/>
-      <c r="L13" s="2"/>
-      <c r="M13" s="2"/>
-      <c r="N13" s="2"/>
-      <c r="O13" s="2"/>
-      <c r="P13" s="2">
+      <c r="L13" s="2">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="Q13" s="3">
-        <f>VLOOKUP(C13,'cost reference'!$B$2:$C$6,2,0)*P13*1.115</f>
+      <c r="M13" s="3">
+        <f>VLOOKUP(C13,'cost reference'!$B$2:$C$8,2,0)*L13</f>
+        <v>18000</v>
+      </c>
+      <c r="N13" s="3">
+        <f t="shared" si="1"/>
         <v>20070</v>
       </c>
-    </row>
-    <row r="14" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="B14" s="2"/>
-      <c r="C14" s="2" t="s">
-        <v>11</v>
-      </c>
+      <c r="V13" s="9"/>
+    </row>
+    <row r="14" spans="2:22" x14ac:dyDescent="0.35">
+      <c r="B14" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" s="5"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
-      <c r="F14" s="2" t="s">
-        <v>15</v>
-      </c>
+      <c r="F14" s="2"/>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
       <c r="L14" s="2"/>
-      <c r="M14" s="2"/>
-      <c r="N14" s="2"/>
-      <c r="O14" s="2"/>
-      <c r="P14" s="2">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="Q14" s="3">
-        <f>VLOOKUP(C14,'cost reference'!$B$2:$C$6,2,0)*P14*1.115</f>
-        <v>15610</v>
-      </c>
-    </row>
-    <row r="15" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="M14" s="3"/>
+      <c r="N14" s="3"/>
+    </row>
+    <row r="15" spans="2:22" x14ac:dyDescent="0.35">
       <c r="B15" s="2"/>
       <c r="C15" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
-      <c r="F15" s="2" t="s">
-        <v>15</v>
-      </c>
+      <c r="F15" s="2"/>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
-      <c r="K15" s="2"/>
-      <c r="L15" s="2"/>
-      <c r="M15" s="2"/>
-      <c r="N15" s="2"/>
-      <c r="O15" s="2"/>
-      <c r="P15" s="2">
+      <c r="K15" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="L15" s="2">
         <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="Q15" s="3">
-        <f>VLOOKUP(C15,'cost reference'!$B$2:$C$6,2,0)*P15*1.115</f>
-        <v>20070</v>
-      </c>
-    </row>
-    <row r="16" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="B16" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C16" s="5"/>
+        <v>5</v>
+      </c>
+      <c r="M15" s="3">
+        <f>VLOOKUP(C15,'cost reference'!$B$2:$C$8,2,0)*L15</f>
+        <v>4500</v>
+      </c>
+      <c r="N15" s="3">
+        <f t="shared" si="1"/>
+        <v>5017.5</v>
+      </c>
+    </row>
+    <row r="16" spans="2:22" x14ac:dyDescent="0.35">
+      <c r="B16" s="2"/>
+      <c r="C16" s="2" t="s">
+        <v>9</v>
+      </c>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
@@ -1096,69 +1177,69 @@
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
-      <c r="K16" s="2"/>
-      <c r="L16" s="2"/>
-      <c r="M16" s="2"/>
-      <c r="N16" s="2"/>
-      <c r="O16" s="2"/>
-      <c r="P16" s="2"/>
-      <c r="Q16" s="3"/>
-    </row>
-    <row r="17" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="B17" s="2"/>
-      <c r="C17" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H17" s="2"/>
-      <c r="I17" s="2"/>
-      <c r="J17" s="2"/>
-      <c r="K17" s="2"/>
-      <c r="L17" s="2"/>
-      <c r="M17" s="2"/>
-      <c r="N17" s="2"/>
-      <c r="O17" s="2"/>
-      <c r="P17" s="2">
-        <v>6</v>
-      </c>
-      <c r="Q17" s="3">
-        <f>VLOOKUP(C17,'cost reference'!$B$2:$C$6,2,0)*P17*1.115</f>
-        <v>6021</v>
-      </c>
-    </row>
-    <row r="18" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="B18" s="2"/>
-      <c r="C18" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H18" s="2"/>
-      <c r="I18" s="2"/>
-      <c r="J18" s="2"/>
-      <c r="K18" s="2"/>
-      <c r="L18" s="2"/>
-      <c r="M18" s="2"/>
-      <c r="N18" s="2"/>
-      <c r="O18" s="2"/>
-      <c r="P18" s="2">
-        <v>6</v>
-      </c>
-      <c r="Q18" s="3">
-        <f>VLOOKUP(C18,'cost reference'!$B$2:$C$6,2,0)*P18*1.115</f>
-        <v>4683</v>
-      </c>
-    </row>
-    <row r="19" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="K16" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="L16" s="2">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="M16" s="3">
+        <f>VLOOKUP(C16,'cost reference'!$B$2:$C$8,2,0)*L16</f>
+        <v>3500</v>
+      </c>
+      <c r="N16" s="3">
+        <f t="shared" si="1"/>
+        <v>3902.5</v>
+      </c>
+    </row>
+    <row r="17" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B17" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="6"/>
+      <c r="J17" s="6"/>
+      <c r="K17" s="6"/>
+      <c r="L17" s="6"/>
+      <c r="M17" s="4">
+        <f>SUM(M5:M16)</f>
+        <v>130000</v>
+      </c>
+      <c r="N17" s="4">
+        <f>SUM(N5:N16)</f>
+        <v>144950</v>
+      </c>
+    </row>
+    <row r="18" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B18" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="6"/>
+      <c r="J18" s="6"/>
+      <c r="K18" s="6"/>
+      <c r="L18" s="6"/>
+      <c r="M18" s="10">
+        <v>0.2</v>
+      </c>
+      <c r="N18" s="4">
+        <f>M18*N17</f>
+        <v>28990</v>
+      </c>
+      <c r="O18" s="9"/>
+    </row>
+    <row r="19" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B19" s="6" t="s">
         <v>17</v>
       </c>
@@ -1172,28 +1253,27 @@
       <c r="J19" s="6"/>
       <c r="K19" s="6"/>
       <c r="L19" s="6"/>
-      <c r="M19" s="6"/>
-      <c r="N19" s="6"/>
-      <c r="O19" s="6"/>
-      <c r="P19" s="6"/>
-      <c r="Q19" s="4">
-        <f>SUM(Q5:Q18)</f>
-        <v>174832</v>
+      <c r="M19" s="1"/>
+      <c r="N19" s="4">
+        <f>N17+N18</f>
+        <v>173940</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="9">
-    <mergeCell ref="Q2:Q3"/>
+  <mergeCells count="11">
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B17:L17"/>
+    <mergeCell ref="N2:N3"/>
+    <mergeCell ref="B18:L18"/>
+    <mergeCell ref="B19:L19"/>
+    <mergeCell ref="B2:C3"/>
+    <mergeCell ref="D2:K2"/>
+    <mergeCell ref="L2:L3"/>
+    <mergeCell ref="M2:M3"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B19:P19"/>
-    <mergeCell ref="B2:C3"/>
-    <mergeCell ref="D2:O2"/>
-    <mergeCell ref="P2:P3"/>
   </mergeCells>
-  <conditionalFormatting sqref="D5:O18">
+  <conditionalFormatting sqref="D5:K16">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>D5&lt;&gt;""</formula>
     </cfRule>

</xml_diff>

<commit_message>
update range of cost overrun
</commit_message>
<xml_diff>
--- a/Gantt.xlsx
+++ b/Gantt.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Monash University LPDP\Study\2024 - Term 5\ITI5057 - Project Management\Assessment 1\Risk Analysis\Monash-PM-Assignment-Monte-Carlo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE7A3EFA-4CB8-439E-95D5-445DAF026F90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F9AEA88-004D-4C38-B9C1-46418792AE1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{0102A14C-CF0C-4EBD-81A6-EA651CF50D0E}"/>
   </bookViews>
@@ -192,6 +192,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -204,8 +206,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -740,7 +740,7 @@
   <dimension ref="B2:V19"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="AK11" sqref="AK11"/>
+      <selection activeCell="A17" sqref="A17:XFD20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -761,33 +761,33 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:22" x14ac:dyDescent="0.35">
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="6" t="s">
+      <c r="C2" s="9"/>
+      <c r="D2" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
-      <c r="L2" s="7" t="s">
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="8"/>
+      <c r="L2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="M2" s="7" t="s">
+      <c r="M2" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="N2" s="7" t="s">
+      <c r="N2" s="9" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="3" spans="2:22" x14ac:dyDescent="0.35">
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
       <c r="D3" s="1">
         <v>1</v>
       </c>
@@ -812,15 +812,15 @@
       <c r="K3" s="1">
         <v>8</v>
       </c>
-      <c r="L3" s="7"/>
-      <c r="M3" s="7"/>
-      <c r="N3" s="7"/>
+      <c r="L3" s="9"/>
+      <c r="M3" s="9"/>
+      <c r="N3" s="9"/>
     </row>
     <row r="4" spans="2:22" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="8"/>
+      <c r="C4" s="10"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
@@ -930,10 +930,10 @@
       </c>
     </row>
     <row r="8" spans="2:22" ht="29.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="8"/>
+      <c r="C8" s="10"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
@@ -979,7 +979,7 @@
         <f t="shared" si="1"/>
         <v>20070</v>
       </c>
-      <c r="V9" s="9"/>
+      <c r="V9" s="5"/>
     </row>
     <row r="10" spans="2:22" x14ac:dyDescent="0.35">
       <c r="B10" s="2"/>
@@ -1014,7 +1014,7 @@
         <f t="shared" si="1"/>
         <v>22300</v>
       </c>
-      <c r="V10" s="9"/>
+      <c r="V10" s="5"/>
     </row>
     <row r="11" spans="2:22" x14ac:dyDescent="0.35">
       <c r="B11" s="2"/>
@@ -1083,7 +1083,7 @@
         <f t="shared" si="1"/>
         <v>15610</v>
       </c>
-      <c r="V12" s="9"/>
+      <c r="V12" s="5"/>
     </row>
     <row r="13" spans="2:22" x14ac:dyDescent="0.35">
       <c r="B13" s="2"/>
@@ -1118,13 +1118,13 @@
         <f t="shared" si="1"/>
         <v>20070</v>
       </c>
-      <c r="V13" s="9"/>
+      <c r="V13" s="5"/>
     </row>
     <row r="14" spans="2:22" x14ac:dyDescent="0.35">
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="C14" s="5"/>
+      <c r="C14" s="7"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
@@ -1194,19 +1194,19 @@
       </c>
     </row>
     <row r="17" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="B17" s="6" t="s">
+      <c r="B17" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="6"/>
-      <c r="G17" s="6"/>
-      <c r="H17" s="6"/>
-      <c r="I17" s="6"/>
-      <c r="J17" s="6"/>
-      <c r="K17" s="6"/>
-      <c r="L17" s="6"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="8"/>
+      <c r="I17" s="8"/>
+      <c r="J17" s="8"/>
+      <c r="K17" s="8"/>
+      <c r="L17" s="8"/>
       <c r="M17" s="4">
         <f>SUM(M5:M16)</f>
         <v>130000</v>
@@ -1217,42 +1217,42 @@
       </c>
     </row>
     <row r="18" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="B18" s="6" t="s">
+      <c r="B18" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="6"/>
-      <c r="H18" s="6"/>
-      <c r="I18" s="6"/>
-      <c r="J18" s="6"/>
-      <c r="K18" s="6"/>
-      <c r="L18" s="6"/>
-      <c r="M18" s="10">
+      <c r="C18" s="8"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="8"/>
+      <c r="G18" s="8"/>
+      <c r="H18" s="8"/>
+      <c r="I18" s="8"/>
+      <c r="J18" s="8"/>
+      <c r="K18" s="8"/>
+      <c r="L18" s="8"/>
+      <c r="M18" s="6">
         <v>0.2</v>
       </c>
       <c r="N18" s="4">
         <f>M18*N17</f>
         <v>28990</v>
       </c>
-      <c r="O18" s="9"/>
+      <c r="O18" s="5"/>
     </row>
     <row r="19" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="B19" s="6" t="s">
+      <c r="B19" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="6"/>
-      <c r="G19" s="6"/>
-      <c r="H19" s="6"/>
-      <c r="I19" s="6"/>
-      <c r="J19" s="6"/>
-      <c r="K19" s="6"/>
-      <c r="L19" s="6"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="8"/>
+      <c r="H19" s="8"/>
+      <c r="I19" s="8"/>
+      <c r="J19" s="8"/>
+      <c r="K19" s="8"/>
+      <c r="L19" s="8"/>
       <c r="M19" s="1"/>
       <c r="N19" s="4">
         <f>N17+N18</f>

</xml_diff>